<commit_message>
updated column name key
</commit_message>
<xml_diff>
--- a/Resources/column name key.xlsx
+++ b/Resources/column name key.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scallina/Desktop/Bootcamp/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scallina/Desktop/Bootcamp/project/RemoteWorkAnalysis/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3800AA1-5264-5F4B-8F83-62671AF9EAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F0E1925-BAF1-694A-957A-53A81B9C2B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="2" xr2:uid="{41571DD3-5495-9840-8B89-93FB721D182E}"/>
+    <workbookView xWindow="32760" yWindow="1040" windowWidth="28800" windowHeight="15940" activeTab="2" xr2:uid="{41571DD3-5495-9840-8B89-93FB721D182E}"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="1" r:id="rId1"/>
     <sheet name="2020" sheetId="2" r:id="rId2"/>
     <sheet name="Merged" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="duplicates" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet2!$A$1:$A$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">duplicates!$A$1:$A$110</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="308">
   <si>
     <t>Response ID</t>
   </si>
@@ -959,13 +959,22 @@
   </si>
   <si>
     <t>Merged Fields</t>
+  </si>
+  <si>
+    <t>Satisfaction</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Identifiers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -976,6 +985,14 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1002,7 +1019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1010,11 +1027,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1355,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD530138-C4FB-C24D-B360-2ADE7CC6311B}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A110"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2254,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D1431F-0874-4B4C-82BF-8D2FB3DE662E}">
   <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2767,95 +2857,185 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F59548-EBA3-2844-B2FE-B5CD1DB227DF}">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A31"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>191</v>
+      </c>
+      <c r="D16" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -2935,7 +3115,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A31">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D10">
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D16">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2946,8 +3147,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:A152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A109"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3713,11 +3914,11 @@
   </sheetData>
   <autoFilter ref="A1:A110" xr:uid="{D7BB569A-B36F-5141-BDDF-FE6FBB07A4CA}">
     <filterColumn colId="0">
-      <colorFilter dxfId="2"/>
+      <colorFilter dxfId="9"/>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>